<commit_message>
Updated attendance sheet for names and the dates currently until the first sprint starts
</commit_message>
<xml_diff>
--- a/Scrum meeting attendance roll-WWIFATM.xlsx
+++ b/Scrum meeting attendance roll-WWIFATM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atm15_000\Documents\GitHub\SDDGroupProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\back up of school files\Software Design &amp; Development\SDDGroupProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Scrum meeting attendance roll</t>
   </si>
@@ -32,18 +32,6 @@
     <t>Team name:</t>
   </si>
   <si>
-    <t>name1 (leader)</t>
-  </si>
-  <si>
-    <t>name4</t>
-  </si>
-  <si>
-    <t>name5</t>
-  </si>
-  <si>
-    <t>name6</t>
-  </si>
-  <si>
     <t>Sprint#</t>
   </si>
   <si>
@@ -71,12 +59,6 @@
     <t>meeting date/time</t>
   </si>
   <si>
-    <t>name7</t>
-  </si>
-  <si>
-    <t>name8</t>
-  </si>
-  <si>
     <t>Sprint0 is for proposal preparation</t>
   </si>
   <si>
@@ -89,16 +71,37 @@
     <t>Michael McGregor</t>
   </si>
   <si>
-    <t>Tuesday / 4:15</t>
-  </si>
-  <si>
-    <t>Saturday / 1:00</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
     <t>Yuchen Feng</t>
+  </si>
+  <si>
+    <t>Ryan Conyac</t>
+  </si>
+  <si>
+    <t>Will McLain</t>
+  </si>
+  <si>
+    <t>Younouss Thiam</t>
+  </si>
+  <si>
+    <t>Brian Davis</t>
+  </si>
+  <si>
+    <t>8/22 / 1:00</t>
+  </si>
+  <si>
+    <t>8/25 / 4:15</t>
+  </si>
+  <si>
+    <t>8/29 / 1:00</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>9/1 / 4:15</t>
   </si>
 </sst>
 </file>
@@ -108,7 +111,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -122,13 +125,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -450,10 +446,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -462,7 +458,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -470,10 +465,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -833,7 +828,7 @@
   <dimension ref="A2:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -844,503 +839,516 @@
     <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.875" customWidth="1"/>
     <col min="6" max="6" width="12.25" customWidth="1"/>
+    <col min="8" max="8" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:11" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19"/>
-    </row>
-    <row r="3" spans="1:11" s="16" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="B2" s="18"/>
+    </row>
+    <row r="3" spans="1:11" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>18</v>
+      <c r="B3" s="16" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="J5" s="6"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19">
+        <v>0</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" s="6" t="s">
+      <c r="I6" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+      <c r="J6" s="26"/>
+      <c r="K6" s="27"/>
+    </row>
+    <row r="7" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19">
         <v>0</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="22" t="s">
+      <c r="B7" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="26"/>
+      <c r="K7" s="27"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="33">
+        <v>0</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="28"/>
-    </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
-        <v>0</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="28"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="34">
-        <v>0</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="22"/>
+      <c r="C8" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="25"/>
+      <c r="I8" s="24"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="9"/>
+      <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="34">
+      <c r="A9" s="33">
         <v>0</v>
       </c>
-      <c r="B9" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="22"/>
+      <c r="B9" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="25"/>
+      <c r="I9" s="24"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="9"/>
+      <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="9">
         <v>1</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="10"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="25"/>
+      <c r="I10" s="24"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="9"/>
+      <c r="K10" s="8"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+      <c r="A11" s="9">
         <v>1</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="10"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="25"/>
+      <c r="I11" s="24"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="9"/>
+      <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
+      <c r="A12" s="9">
         <v>1</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="10"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="9"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="25"/>
+      <c r="I12" s="24"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="9"/>
+      <c r="K12" s="8"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+      <c r="A13" s="9">
         <v>1</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="10"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="25"/>
+      <c r="I13" s="24"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="9"/>
+      <c r="K13" s="8"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
+      <c r="A14" s="9">
         <v>2</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="10"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="9"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="25"/>
+      <c r="I14" s="24"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="9"/>
+      <c r="K14" s="8"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="A15" s="9">
         <v>2</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="10"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="25"/>
+      <c r="I15" s="24"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="9"/>
+      <c r="K15" s="8"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+      <c r="A16" s="9">
         <v>2</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="10"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="9"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="25"/>
+      <c r="I16" s="24"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="9"/>
+      <c r="K16" s="8"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
+      <c r="A17" s="9">
         <v>2</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="10"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="9"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="25"/>
+      <c r="I17" s="24"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="9"/>
+      <c r="K17" s="8"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="A18" s="9">
         <v>3</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="10"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="9"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="25"/>
+      <c r="I18" s="24"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="9"/>
+      <c r="K18" s="8"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
+      <c r="A19" s="9">
         <v>3</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="10"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="25"/>
+      <c r="I19" s="24"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="9"/>
+      <c r="K19" s="8"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
+      <c r="A20" s="9">
         <v>3</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="10"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="9"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="25"/>
+      <c r="I20" s="24"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="9"/>
+      <c r="K20" s="8"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
+      <c r="A21" s="9">
         <v>3</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="10"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="9"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="25"/>
+      <c r="I21" s="24"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="9"/>
+      <c r="K21" s="8"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
+      <c r="A22" s="9">
         <v>4</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="10"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="9"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="25"/>
+      <c r="I22" s="24"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="9"/>
+      <c r="K22" s="8"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
+      <c r="A23" s="9">
         <v>4</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="10"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="9"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="25"/>
+      <c r="I23" s="24"/>
       <c r="J23" s="2"/>
-      <c r="K23" s="9"/>
+      <c r="K23" s="8"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+      <c r="A24" s="9">
         <v>4</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="10"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="9"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="25"/>
+      <c r="I24" s="24"/>
       <c r="J24" s="2"/>
-      <c r="K24" s="9"/>
+      <c r="K24" s="8"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
+      <c r="A25" s="9">
         <v>4</v>
       </c>
       <c r="B25" s="3"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="10"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="9"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="25"/>
+      <c r="I25" s="24"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="9"/>
+      <c r="K25" s="8"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
+      <c r="A26" s="9">
         <v>5</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="10"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="9"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
-      <c r="I26" s="25"/>
+      <c r="I26" s="24"/>
       <c r="J26" s="2"/>
-      <c r="K26" s="9"/>
+      <c r="K26" s="8"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
+      <c r="A27" s="9">
         <v>5</v>
       </c>
       <c r="B27" s="3"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="10"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="9"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="25"/>
+      <c r="I27" s="24"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="9"/>
+      <c r="K27" s="8"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
+      <c r="A28" s="9">
         <v>5</v>
       </c>
       <c r="B28" s="3"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="10"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="9"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="I28" s="25"/>
+      <c r="I28" s="24"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="9"/>
+      <c r="K28" s="8"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
+      <c r="A29" s="9">
         <v>5</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="10"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="9"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-      <c r="I29" s="25"/>
+      <c r="I29" s="24"/>
       <c r="J29" s="2"/>
-      <c r="K29" s="9"/>
+      <c r="K29" s="8"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="33"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="32"/>
     </row>
     <row r="31" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="11"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="13"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="12"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated for today's meeting
</commit_message>
<xml_diff>
--- a/Scrum meeting attendance roll-WWIFATM.xlsx
+++ b/Scrum meeting attendance roll-WWIFATM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>Scrum meeting attendance roll</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>9/1 / 4:15</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
@@ -827,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -964,12 +967,24 @@
       <c r="C8" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="24"/>
+      <c r="D8" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>26</v>
+      </c>
       <c r="J8" s="2"/>
       <c r="K8" s="8"/>
     </row>

</xml_diff>

<commit_message>
Edited backlog to fix formatting updated attendance for 9/1 added workload distribution sheet for proposal
</commit_message>
<xml_diff>
--- a/Scrum meeting attendance roll-WWIFATM.xlsx
+++ b/Scrum meeting attendance roll-WWIFATM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuchen\Documents\GitHub\SDDGroupProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\back up of school files\Software Design &amp; Development\SDDGroupProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>Scrum meeting attendance roll</t>
   </si>
@@ -98,13 +98,13 @@
     <t>8/29 / 1:00</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>9/1 / 4:15</t>
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
   </si>
 </sst>
 </file>
@@ -134,6 +134,7 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -141,6 +142,7 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -831,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -919,7 +921,7 @@
         <v>15</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I6" s="23" t="s">
         <v>15</v>
@@ -953,7 +955,7 @@
         <v>15</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J7" s="26"/>
       <c r="K7" s="27"/>
@@ -984,7 +986,7 @@
         <v>15</v>
       </c>
       <c r="I8" s="34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="8"/>
@@ -994,17 +996,29 @@
         <v>0</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="24"/>
+      <c r="D9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="J9" s="2"/>
       <c r="K9" s="8"/>
     </row>

</xml_diff>

<commit_message>
Created some tile sets and tested out using that in the background panel. Updated some of the sizing for the panel and main jframe to test out with the background sizing. Updated attendance sheet for 9/8
</commit_message>
<xml_diff>
--- a/Scrum meeting attendance roll-WWIFATM.xlsx
+++ b/Scrum meeting attendance roll-WWIFATM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
   <si>
     <t>Scrum meeting attendance roll</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>9/5 /4:15</t>
+  </si>
+  <si>
+    <t>9/8/ 4:15</t>
   </si>
 </sst>
 </file>
@@ -837,7 +840,7 @@
   <dimension ref="A2:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1060,14 +1063,30 @@
       <c r="A11" s="9">
         <v>1</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="24"/>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="J11" s="2"/>
       <c r="K11" s="8"/>
     </row>

</xml_diff>

<commit_message>
Changes to the save data class and starting the leaderboard panel
</commit_message>
<xml_diff>
--- a/Scrum meeting attendance roll-WWIFATM.xlsx
+++ b/Scrum meeting attendance roll-WWIFATM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="30">
   <si>
     <t>Scrum meeting attendance roll</t>
   </si>
@@ -107,10 +107,13 @@
     <t>U</t>
   </si>
   <si>
-    <t>9/5 /4:15</t>
-  </si>
-  <si>
     <t>9/8/ 4:15</t>
+  </si>
+  <si>
+    <t>9/5 /1:00</t>
+  </si>
+  <si>
+    <t>9/12 /1:00</t>
   </si>
 </sst>
 </file>
@@ -839,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1033,7 +1036,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="23" t="s">
         <v>13</v>
@@ -1064,7 +1067,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="23" t="s">
         <v>13</v>
@@ -1094,14 +1097,30 @@
       <c r="A12" s="9">
         <v>1</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="24"/>
+      <c r="B12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="J12" s="2"/>
       <c r="K12" s="8"/>
     </row>

</xml_diff>

<commit_message>
updated log, contribution log updated, attendance updated, test text for the save data added to read more scores into the leader board, removed un-needed classes, integrated younouss's keycontroller class into the ship, updated leaderboard to correct for array size issue
</commit_message>
<xml_diff>
--- a/Scrum meeting attendance roll-WWIFATM.xlsx
+++ b/Scrum meeting attendance roll-WWIFATM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="31">
   <si>
     <t>Scrum meeting attendance roll</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>9/12 /1:00</t>
+  </si>
+  <si>
+    <t>9/15 /4:15</t>
   </si>
 </sst>
 </file>
@@ -842,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1128,14 +1131,30 @@
       <c r="A13" s="9">
         <v>1</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="24"/>
+      <c r="B13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="J13" s="2"/>
       <c r="K13" s="8"/>
     </row>

</xml_diff>

<commit_message>
updated attendance for today, marked completed items in the backlog, updated the sprint backlog, updated the contribution log
</commit_message>
<xml_diff>
--- a/Scrum meeting attendance roll-WWIFATM.xlsx
+++ b/Scrum meeting attendance roll-WWIFATM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="32">
   <si>
     <t>Scrum meeting attendance roll</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>9/15 /4:15</t>
+  </si>
+  <si>
+    <t>9/19 / 1:00</t>
   </si>
 </sst>
 </file>
@@ -846,7 +849,7 @@
   <dimension ref="A2:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1162,14 +1165,30 @@
       <c r="A14" s="9">
         <v>2</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="24"/>
+      <c r="B14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="J14" s="2"/>
       <c r="K14" s="8"/>
     </row>

</xml_diff>

<commit_message>
Updated attendance roll, created enemy class
</commit_message>
<xml_diff>
--- a/Scrum meeting attendance roll-WWIFATM.xlsx
+++ b/Scrum meeting attendance roll-WWIFATM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="33">
   <si>
     <t>Scrum meeting attendance roll</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>9/19 / 1:00</t>
+  </si>
+  <si>
+    <t>9/22 / 4:15</t>
   </si>
 </sst>
 </file>
@@ -848,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1196,14 +1199,30 @@
       <c r="A15" s="9">
         <v>2</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="24"/>
+      <c r="B15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="J15" s="2"/>
       <c r="K15" s="8"/>
     </row>

</xml_diff>

<commit_message>
updated some notes for the backlog, updated attendance for 9/29, cleared out temp files that didn't need to be in the directory
</commit_message>
<xml_diff>
--- a/Scrum meeting attendance roll-WWIFATM.xlsx
+++ b/Scrum meeting attendance roll-WWIFATM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="35">
   <si>
     <t>Scrum meeting attendance roll</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>9/26 /1:00</t>
+  </si>
+  <si>
+    <t>9/29 / 4:15</t>
   </si>
 </sst>
 </file>
@@ -854,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1264,14 +1267,30 @@
       <c r="A17" s="9">
         <v>2</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="24"/>
+      <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="J17" s="2"/>
       <c r="K17" s="8"/>
     </row>

</xml_diff>

<commit_message>
Backlog and other things updated for the start of the sprint
</commit_message>
<xml_diff>
--- a/Scrum meeting attendance roll-WWIFATM.xlsx
+++ b/Scrum meeting attendance roll-WWIFATM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="36">
   <si>
     <t>Scrum meeting attendance roll</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>9/29 / 4:15</t>
+  </si>
+  <si>
+    <t>10/3 /1:00</t>
   </si>
 </sst>
 </file>
@@ -857,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1298,14 +1301,30 @@
       <c r="A18" s="9">
         <v>3</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="24"/>
+      <c r="B18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="J18" s="2"/>
       <c r="K18" s="8"/>
     </row>

</xml_diff>

<commit_message>
added flyweight for use for ships, updated attendance for 10/6
</commit_message>
<xml_diff>
--- a/Scrum meeting attendance roll-WWIFATM.xlsx
+++ b/Scrum meeting attendance roll-WWIFATM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="37">
   <si>
     <t>Scrum meeting attendance roll</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>10/3 /1:00</t>
+  </si>
+  <si>
+    <t>10/6 / 4:15</t>
   </si>
 </sst>
 </file>
@@ -861,7 +864,7 @@
   <dimension ref="A2:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1332,14 +1335,30 @@
       <c r="A19" s="9">
         <v>3</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="24"/>
+      <c r="B19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="J19" s="2"/>
       <c r="K19" s="8"/>
     </row>

</xml_diff>

<commit_message>
hopefully fixed some major bugs for the enemies, collision is not working for them currently
</commit_message>
<xml_diff>
--- a/Scrum meeting attendance roll-WWIFATM.xlsx
+++ b/Scrum meeting attendance roll-WWIFATM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="38">
   <si>
     <t>Scrum meeting attendance roll</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>10/6 / 4:15</t>
+  </si>
+  <si>
+    <t>10/10 /1:00</t>
   </si>
 </sst>
 </file>
@@ -863,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1366,14 +1369,30 @@
       <c r="A20" s="9">
         <v>3</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="24"/>
+      <c r="B20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="J20" s="2"/>
       <c r="K20" s="8"/>
     </row>

</xml_diff>

<commit_message>
attendance for 10/13 and some fixes for enemy collisions
</commit_message>
<xml_diff>
--- a/Scrum meeting attendance roll-WWIFATM.xlsx
+++ b/Scrum meeting attendance roll-WWIFATM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="39">
   <si>
     <t>Scrum meeting attendance roll</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>10/10 /1:00</t>
+  </si>
+  <si>
+    <t>10/13 / 4:15</t>
   </si>
 </sst>
 </file>
@@ -866,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1400,14 +1403,30 @@
       <c r="A21" s="9">
         <v>3</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="24"/>
+      <c r="B21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="J21" s="2"/>
       <c r="K21" s="8"/>
     </row>

</xml_diff>

<commit_message>
hopefully things are fixed
</commit_message>
<xml_diff>
--- a/Scrum meeting attendance roll-WWIFATM.xlsx
+++ b/Scrum meeting attendance roll-WWIFATM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="40">
   <si>
     <t>Scrum meeting attendance roll</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>10/13 / 4:15</t>
+  </si>
+  <si>
+    <t>10/16 /1:00</t>
   </si>
 </sst>
 </file>
@@ -869,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1434,14 +1437,30 @@
       <c r="A22" s="9">
         <v>4</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="24"/>
+      <c r="B22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="J22" s="2"/>
       <c r="K22" s="8"/>
     </row>
@@ -1450,7 +1469,9 @@
         <v>4</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="24"/>
+      <c r="C23" s="23" t="s">
+        <v>13</v>
+      </c>
       <c r="D23" s="9"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -1465,7 +1486,9 @@
         <v>4</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="24"/>
+      <c r="C24" s="23" t="s">
+        <v>13</v>
+      </c>
       <c r="D24" s="9"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1480,7 +1503,9 @@
         <v>4</v>
       </c>
       <c r="B25" s="3"/>
-      <c r="C25" s="24"/>
+      <c r="C25" s="23" t="s">
+        <v>13</v>
+      </c>
       <c r="D25" s="9"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>

</xml_diff>

<commit_message>
updated the backlog for typos, updated attendance for 10/20, updated enemies to have more randomization
</commit_message>
<xml_diff>
--- a/Scrum meeting attendance roll-WWIFATM.xlsx
+++ b/Scrum meeting attendance roll-WWIFATM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="41">
   <si>
     <t>Scrum meeting attendance roll</t>
   </si>
@@ -143,7 +143,10 @@
     <t>10/13 / 4:15</t>
   </si>
   <si>
-    <t>10/16 /1:00</t>
+    <t>10/17 /1:00</t>
+  </si>
+  <si>
+    <t>10/20 /4:15</t>
   </si>
 </sst>
 </file>
@@ -872,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1468,16 +1471,30 @@
       <c r="A23" s="9">
         <v>4</v>
       </c>
-      <c r="B23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="C23" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="24"/>
+      <c r="D23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="J23" s="2"/>
       <c r="K23" s="8"/>
     </row>

</xml_diff>

<commit_message>
level seems to be working on the transition attendance for 11/3
</commit_message>
<xml_diff>
--- a/Scrum meeting attendance roll-WWIFATM.xlsx
+++ b/Scrum meeting attendance roll-WWIFATM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="45">
   <si>
     <t>Scrum meeting attendance roll</t>
   </si>
@@ -155,7 +155,10 @@
     <t>10/27 /4:15</t>
   </si>
   <si>
-    <t>10/31 1/:00</t>
+    <t>10/31 /1:00</t>
+  </si>
+  <si>
+    <t>11/3 /4:15</t>
   </si>
 </sst>
 </file>
@@ -505,7 +508,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -541,6 +544,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -885,7 +889,7 @@
   <dimension ref="A2:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1573,7 +1577,7 @@
       <c r="A26" s="9">
         <v>5</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="35" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="23" t="s">
@@ -1604,14 +1608,30 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="24"/>
+      <c r="B27" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="J27" s="2"/>
       <c r="K27" s="8"/>
     </row>
@@ -1620,7 +1640,9 @@
         <v>5</v>
       </c>
       <c r="B28" s="3"/>
-      <c r="C28" s="24"/>
+      <c r="C28" s="23" t="s">
+        <v>13</v>
+      </c>
       <c r="D28" s="9"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -1635,7 +1657,9 @@
         <v>5</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="24"/>
+      <c r="C29" s="23" t="s">
+        <v>13</v>
+      </c>
       <c r="D29" s="9"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>

</xml_diff>

<commit_message>
backlog, attendance, team contribution all updated
</commit_message>
<xml_diff>
--- a/Scrum meeting attendance roll-WWIFATM.xlsx
+++ b/Scrum meeting attendance roll-WWIFATM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\back up of school files\Software Design &amp; Development\SDDGroupProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\SDDGroupProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="53">
   <si>
     <t>Scrum meeting attendance roll</t>
   </si>
@@ -177,12 +177,18 @@
   </si>
   <si>
     <t>11/24 /4:15</t>
+  </si>
+  <si>
+    <t>11/28 /1:00</t>
+  </si>
+  <si>
+    <t>12/1 /4:15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -242,7 +248,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -341,21 +347,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -508,23 +499,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -535,7 +513,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -548,33 +526,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -916,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K39"/>
+  <dimension ref="A2:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -933,17 +910,17 @@
     <col min="8" max="8" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:11" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18"/>
-    </row>
-    <row r="3" spans="1:11" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="B2" s="16"/>
+    </row>
+    <row r="3" spans="1:11" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="14" t="s">
         <v>12</v>
       </c>
     </row>
@@ -956,10 +933,10 @@
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -977,119 +954,119 @@
       <c r="H5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="20" t="s">
         <v>20</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19">
+      <c r="A6" s="17">
         <v>0</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="21" t="s">
+      <c r="C6" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="25"/>
-      <c r="K6" s="26"/>
+      <c r="I6" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="23"/>
+      <c r="K6" s="24"/>
     </row>
     <row r="7" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
+      <c r="A7" s="17">
         <v>0</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="23" t="s">
+      <c r="C7" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="25"/>
-      <c r="K7" s="26"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="24"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="31">
+      <c r="A8" s="29">
         <v>0</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="33" t="s">
+      <c r="C8" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="31" t="s">
         <v>25</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="31">
+      <c r="A9" s="29">
         <v>0</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -1101,7 +1078,7 @@
       <c r="H9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J9" s="2"/>
@@ -1114,7 +1091,7 @@
       <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="9" t="s">
@@ -1132,7 +1109,7 @@
       <c r="H10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J10" s="2"/>
@@ -1145,7 +1122,7 @@
       <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="9" t="s">
@@ -1163,7 +1140,7 @@
       <c r="H11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="24" t="s">
+      <c r="I11" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J11" s="2"/>
@@ -1176,7 +1153,7 @@
       <c r="B12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="9" t="s">
@@ -1194,7 +1171,7 @@
       <c r="H12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J12" s="2"/>
@@ -1207,7 +1184,7 @@
       <c r="B13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -1225,7 +1202,7 @@
       <c r="H13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="24" t="s">
+      <c r="I13" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J13" s="2"/>
@@ -1238,7 +1215,7 @@
       <c r="B14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="9" t="s">
@@ -1256,7 +1233,7 @@
       <c r="H14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="24" t="s">
+      <c r="I14" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J14" s="2"/>
@@ -1269,7 +1246,7 @@
       <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="9" t="s">
@@ -1287,7 +1264,7 @@
       <c r="H15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="24" t="s">
+      <c r="I15" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J15" s="2"/>
@@ -1300,7 +1277,7 @@
       <c r="B16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="9" t="s">
@@ -1318,7 +1295,7 @@
       <c r="H16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="24" t="s">
+      <c r="I16" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J16" s="2"/>
@@ -1331,7 +1308,7 @@
       <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="9" t="s">
@@ -1349,7 +1326,7 @@
       <c r="H17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="24" t="s">
+      <c r="I17" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J17" s="2"/>
@@ -1362,7 +1339,7 @@
       <c r="B18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="9" t="s">
@@ -1380,7 +1357,7 @@
       <c r="H18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="24" t="s">
+      <c r="I18" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J18" s="2"/>
@@ -1393,7 +1370,7 @@
       <c r="B19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="9" t="s">
@@ -1411,7 +1388,7 @@
       <c r="H19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="24" t="s">
+      <c r="I19" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J19" s="2"/>
@@ -1424,7 +1401,7 @@
       <c r="B20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="9" t="s">
@@ -1442,7 +1419,7 @@
       <c r="H20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="24" t="s">
+      <c r="I20" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J20" s="2"/>
@@ -1455,7 +1432,7 @@
       <c r="B21" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="9" t="s">
@@ -1473,7 +1450,7 @@
       <c r="H21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I21" s="24" t="s">
+      <c r="I21" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J21" s="2"/>
@@ -1486,7 +1463,7 @@
       <c r="B22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="9" t="s">
@@ -1504,7 +1481,7 @@
       <c r="H22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I22" s="24" t="s">
+      <c r="I22" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J22" s="2"/>
@@ -1517,7 +1494,7 @@
       <c r="B23" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="9" t="s">
@@ -1535,7 +1512,7 @@
       <c r="H23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I23" s="24" t="s">
+      <c r="I23" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J23" s="2"/>
@@ -1548,7 +1525,7 @@
       <c r="B24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="9" t="s">
@@ -1566,7 +1543,7 @@
       <c r="H24" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I24" s="24" t="s">
+      <c r="I24" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J24" s="2"/>
@@ -1579,7 +1556,7 @@
       <c r="B25" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="9" t="s">
@@ -1597,7 +1574,7 @@
       <c r="H25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I25" s="24" t="s">
+      <c r="I25" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J25" s="2"/>
@@ -1607,10 +1584,10 @@
       <c r="A26" s="9">
         <v>5</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="9" t="s">
@@ -1628,7 +1605,7 @@
       <c r="H26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="24" t="s">
+      <c r="I26" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J26" s="2"/>
@@ -1638,10 +1615,10 @@
       <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="9" t="s">
@@ -1659,7 +1636,7 @@
       <c r="H27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I27" s="24" t="s">
+      <c r="I27" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J27" s="2"/>
@@ -1672,7 +1649,7 @@
       <c r="B28" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -1690,7 +1667,7 @@
       <c r="H28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I28" s="24" t="s">
+      <c r="I28" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J28" s="2"/>
@@ -1703,7 +1680,7 @@
       <c r="B29" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="9" t="s">
@@ -1721,7 +1698,7 @@
       <c r="H29" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I29" s="24" t="s">
+      <c r="I29" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J29" s="2"/>
@@ -1732,58 +1709,58 @@
       <c r="B30" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="G30" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="28"/>
-      <c r="I30" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="J30" s="28"/>
-      <c r="K30" s="30"/>
+      <c r="C30" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="26"/>
+      <c r="I30" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="26"/>
+      <c r="K30" s="28"/>
     </row>
     <row r="31" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="14" t="s">
+      <c r="A31" s="25"/>
+      <c r="B31" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J31" s="11"/>
-      <c r="K31" s="12"/>
+      <c r="C31" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="10"/>
+      <c r="K31" s="11"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="35"/>
-      <c r="B32" s="36" t="s">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C32" s="23" t="s">
@@ -1792,25 +1769,25 @@
       <c r="D32" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="F32" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="H32" s="35"/>
-      <c r="I32" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
+      <c r="E32" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="2"/>
+      <c r="I32" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
-      <c r="B33" s="36" t="s">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C33" s="23" t="s">
@@ -1819,47 +1796,111 @@
       <c r="D33" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="G33" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="35"/>
-      <c r="I33" s="38" t="s">
+      <c r="E33" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="2"/>
+      <c r="I33" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="J33" s="35"/>
-      <c r="K33" s="35"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="2"/>
+      <c r="I34" s="37" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="2"/>
+      <c r="I35" s="37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="I36" s="34"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="34"/>
+      <c r="I37" s="34"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>